<commit_message>
Updated csv to excel automation file and readme.md file.
</commit_message>
<xml_diff>
--- a/05-automation-projects/02-csv-excel-automation/clean_sales_report.xlsx
+++ b/05-automation-projects/02-csv-excel-automation/clean_sales_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>CustomerName</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -447,11 +447,6 @@
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Amount</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>City</t>
         </is>
       </c>
     </row>
@@ -469,11 +464,6 @@
       <c r="C2" t="n">
         <v>50000</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Delhi</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -489,11 +479,6 @@
       <c r="C3" t="n">
         <v>20000</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Mumbai</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -504,11 +489,6 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
         <v>30000</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Kolkata</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>